<commit_message>
Form 8 Annual Config Updated
</commit_message>
<xml_diff>
--- a/Config Files/FORM-8(ANNUAL)_nodes_config.xlsx
+++ b/Config Files/FORM-8(ANNUAL)_nodes_config.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MCA Portal\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mns-admin\Documents\Python\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{518F01C8-BC84-466E-A70B-262A27FE8EA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11D3020D-4551-4060-AF56-27C790302483}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="931" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="931" uniqueCount="218">
   <si>
     <t>Field_Name</t>
   </si>
@@ -404,9 +404,6 @@
     <t>total_other_expenses</t>
   </si>
   <si>
-    <t>Formula</t>
-  </si>
-  <si>
     <t>other_expenses+power_and_fuel+administrative_expenses+payment_to_auditors+selling_expenses+insurance_expenses</t>
   </si>
   <si>
@@ -611,9 +608,6 @@
     <t>membership_number</t>
   </si>
   <si>
-    <t>MEMBERSHIP_NO</t>
-  </si>
-  <si>
     <t>id</t>
   </si>
   <si>
@@ -678,6 +672,9 @@
   </si>
   <si>
     <t>null</t>
+  </si>
+  <si>
+    <t>DPIN_INTPAN_MEM</t>
   </si>
 </sst>
 </file>
@@ -2191,8 +2188,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I127"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A98" workbookViewId="0">
+      <selection activeCell="E126" sqref="E126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3682,7 +3679,7 @@
         <v>16</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="E61" s="2" t="s">
         <v>102</v>
@@ -3709,7 +3706,7 @@
         <v>16</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="E62" s="2" t="s">
         <v>105</v>
@@ -3736,7 +3733,7 @@
         <v>16</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="E63" s="2" t="s">
         <v>107</v>
@@ -3763,7 +3760,7 @@
         <v>16</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="E64" s="2" t="s">
         <v>109</v>
@@ -3790,7 +3787,7 @@
         <v>16</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="E65" s="2" t="s">
         <v>111</v>
@@ -3817,7 +3814,7 @@
         <v>16</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="E66" s="2" t="s">
         <v>113</v>
@@ -3844,7 +3841,7 @@
         <v>16</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="E67" s="2" t="s">
         <v>115</v>
@@ -3871,7 +3868,7 @@
         <v>16</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="E68" s="2" t="s">
         <v>117</v>
@@ -3898,7 +3895,7 @@
         <v>16</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="E69" s="2" t="s">
         <v>119</v>
@@ -3925,7 +3922,7 @@
         <v>16</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="E70" s="2" t="s">
         <v>122</v>
@@ -3952,7 +3949,7 @@
         <v>16</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="E71" s="2" t="s">
         <v>125</v>
@@ -3979,10 +3976,10 @@
         <v>16</v>
       </c>
       <c r="D72" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E72" s="29" t="s">
         <v>127</v>
-      </c>
-      <c r="E72" s="29" t="s">
-        <v>128</v>
       </c>
       <c r="F72" s="19" t="s">
         <v>14</v>
@@ -3997,7 +3994,7 @@
     </row>
     <row r="73" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B73" s="2" t="s">
         <v>9</v>
@@ -4006,10 +4003,10 @@
         <v>16</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>127</v>
+        <v>25</v>
       </c>
       <c r="E73" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F73" s="19" t="s">
         <v>14</v>
@@ -4018,13 +4015,13 @@
         <v>103</v>
       </c>
       <c r="H73" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I73" s="5"/>
     </row>
     <row r="74" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B74" s="2" t="s">
         <v>9</v>
@@ -4033,10 +4030,10 @@
         <v>16</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F74" s="19" t="s">
         <v>14</v>
@@ -4045,13 +4042,13 @@
         <v>103</v>
       </c>
       <c r="H74" s="10" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="I74" s="5"/>
     </row>
     <row r="75" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B75" s="2" t="s">
         <v>9</v>
@@ -4060,10 +4057,10 @@
         <v>16</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F75" s="19" t="s">
         <v>14</v>
@@ -4072,13 +4069,13 @@
         <v>103</v>
       </c>
       <c r="H75" s="10" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I75" s="5"/>
     </row>
     <row r="76" spans="1:9" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B76" s="2" t="s">
         <v>9</v>
@@ -4087,10 +4084,10 @@
         <v>16</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>127</v>
+        <v>25</v>
       </c>
       <c r="E76" s="29" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F76" s="19" t="s">
         <v>14</v>
@@ -4099,13 +4096,13 @@
         <v>103</v>
       </c>
       <c r="H76" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I76" s="5"/>
     </row>
     <row r="77" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B77" s="2" t="s">
         <v>9</v>
@@ -4114,10 +4111,10 @@
         <v>16</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="E77" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F77" s="19" t="s">
         <v>14</v>
@@ -4126,13 +4123,13 @@
         <v>103</v>
       </c>
       <c r="H77" s="10" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="I77" s="5"/>
     </row>
     <row r="78" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="8" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B78" s="2" t="s">
         <v>9</v>
@@ -4141,10 +4138,10 @@
         <v>16</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>127</v>
+        <v>25</v>
       </c>
       <c r="E78" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F78" s="19" t="s">
         <v>14</v>
@@ -4153,13 +4150,13 @@
         <v>103</v>
       </c>
       <c r="H78" s="8" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="I78" s="5"/>
     </row>
     <row r="79" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B79" s="2" t="s">
         <v>9</v>
@@ -4168,10 +4165,10 @@
         <v>16</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="E79" s="30" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F79" s="19" t="s">
         <v>14</v>
@@ -4180,13 +4177,13 @@
         <v>103</v>
       </c>
       <c r="H79" s="10" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="I79" s="5"/>
     </row>
     <row r="80" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B80" s="2" t="s">
         <v>9</v>
@@ -4195,10 +4192,10 @@
         <v>16</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="E80" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F80" s="21" t="s">
         <v>14</v>
@@ -4207,7 +4204,7 @@
         <v>103</v>
       </c>
       <c r="H80" s="10" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="I80" s="5"/>
     </row>
@@ -4226,7 +4223,7 @@
     </row>
     <row r="82" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="25" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B82" s="5"/>
       <c r="C82" s="5"/>
@@ -4248,10 +4245,10 @@
         <v>21</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="E83" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F83" s="17" t="s">
         <v>14</v>
@@ -4275,10 +4272,10 @@
         <v>21</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="E84" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F84" s="19" t="s">
         <v>14</v>
@@ -4302,10 +4299,10 @@
         <v>21</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="E85" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F85" s="19" t="s">
         <v>14</v>
@@ -4329,10 +4326,10 @@
         <v>21</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="E86" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F86" s="19" t="s">
         <v>14</v>
@@ -4356,10 +4353,10 @@
         <v>21</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="E87" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F87" s="19" t="s">
         <v>14</v>
@@ -4383,10 +4380,10 @@
         <v>21</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="E88" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F88" s="19" t="s">
         <v>14</v>
@@ -4395,7 +4392,7 @@
         <v>103</v>
       </c>
       <c r="H88" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="I88" s="5"/>
     </row>
@@ -4410,10 +4407,10 @@
         <v>21</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="E89" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F89" s="19" t="s">
         <v>14</v>
@@ -4422,7 +4419,7 @@
         <v>103</v>
       </c>
       <c r="H89" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="I89" s="5"/>
     </row>
@@ -4437,10 +4434,10 @@
         <v>21</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="E90" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F90" s="19" t="s">
         <v>14</v>
@@ -4449,7 +4446,7 @@
         <v>103</v>
       </c>
       <c r="H90" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I90" s="5"/>
     </row>
@@ -4464,10 +4461,10 @@
         <v>21</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="E91" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F91" s="19" t="s">
         <v>14</v>
@@ -4491,10 +4488,10 @@
         <v>21</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="E92" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F92" s="19" t="s">
         <v>14</v>
@@ -4518,10 +4515,10 @@
         <v>21</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="E93" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F93" s="19" t="s">
         <v>14</v>
@@ -4530,7 +4527,7 @@
         <v>103</v>
       </c>
       <c r="H93" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I93" s="5"/>
     </row>
@@ -4545,10 +4542,10 @@
         <v>21</v>
       </c>
       <c r="D94" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E94" s="29" t="s">
         <v>127</v>
-      </c>
-      <c r="E94" s="29" t="s">
-        <v>128</v>
       </c>
       <c r="F94" s="19" t="s">
         <v>14</v>
@@ -4563,7 +4560,7 @@
     </row>
     <row r="95" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B95" s="2" t="s">
         <v>9</v>
@@ -4572,10 +4569,10 @@
         <v>21</v>
       </c>
       <c r="D95" s="2" t="s">
-        <v>127</v>
+        <v>25</v>
       </c>
       <c r="E95" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F95" s="19" t="s">
         <v>14</v>
@@ -4584,13 +4581,13 @@
         <v>103</v>
       </c>
       <c r="H95" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I95" s="5"/>
     </row>
     <row r="96" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B96" s="2" t="s">
         <v>9</v>
@@ -4599,10 +4596,10 @@
         <v>21</v>
       </c>
       <c r="D96" s="2" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="E96" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F96" s="19" t="s">
         <v>14</v>
@@ -4611,13 +4608,13 @@
         <v>103</v>
       </c>
       <c r="H96" s="10" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="I96" s="5"/>
     </row>
     <row r="97" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B97" s="2" t="s">
         <v>9</v>
@@ -4626,10 +4623,10 @@
         <v>21</v>
       </c>
       <c r="D97" s="2" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="E97" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F97" s="19" t="s">
         <v>14</v>
@@ -4638,13 +4635,13 @@
         <v>103</v>
       </c>
       <c r="H97" s="10" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I97" s="5"/>
     </row>
     <row r="98" spans="1:9" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B98" s="2" t="s">
         <v>9</v>
@@ -4653,10 +4650,10 @@
         <v>21</v>
       </c>
       <c r="D98" s="2" t="s">
-        <v>127</v>
+        <v>25</v>
       </c>
       <c r="E98" s="29" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F98" s="19" t="s">
         <v>14</v>
@@ -4665,13 +4662,13 @@
         <v>103</v>
       </c>
       <c r="H98" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I98" s="5"/>
     </row>
     <row r="99" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B99" s="2" t="s">
         <v>9</v>
@@ -4680,10 +4677,10 @@
         <v>21</v>
       </c>
       <c r="D99" s="2" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="E99" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F99" s="19" t="s">
         <v>14</v>
@@ -4692,13 +4689,13 @@
         <v>103</v>
       </c>
       <c r="H99" s="10" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="I99" s="5"/>
     </row>
     <row r="100" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="8" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B100" s="2" t="s">
         <v>9</v>
@@ -4707,10 +4704,10 @@
         <v>21</v>
       </c>
       <c r="D100" s="2" t="s">
-        <v>127</v>
+        <v>25</v>
       </c>
       <c r="E100" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F100" s="19" t="s">
         <v>14</v>
@@ -4719,13 +4716,13 @@
         <v>103</v>
       </c>
       <c r="H100" s="8" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="I100" s="5"/>
     </row>
     <row r="101" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B101" s="2" t="s">
         <v>9</v>
@@ -4734,10 +4731,10 @@
         <v>21</v>
       </c>
       <c r="D101" s="2" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="E101" s="30" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F101" s="19" t="s">
         <v>14</v>
@@ -4746,13 +4743,13 @@
         <v>103</v>
       </c>
       <c r="H101" s="10" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="I101" s="5"/>
     </row>
     <row r="102" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B102" s="2" t="s">
         <v>9</v>
@@ -4761,10 +4758,10 @@
         <v>21</v>
       </c>
       <c r="D102" s="2" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="E102" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F102" s="19" t="s">
         <v>14</v>
@@ -4773,13 +4770,13 @@
         <v>103</v>
       </c>
       <c r="H102" s="10" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="I102" s="5"/>
     </row>
     <row r="103" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="15" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B103" s="5"/>
       <c r="C103" s="5"/>
@@ -4792,7 +4789,7 @@
     </row>
     <row r="104" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="10" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B104" s="2" t="s">
         <v>9</v>
@@ -4804,22 +4801,22 @@
         <v>25</v>
       </c>
       <c r="E104" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="F104" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="G104" s="33" t="s">
         <v>168</v>
       </c>
-      <c r="F104" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="G104" s="33" t="s">
-        <v>169</v>
-      </c>
       <c r="H104" s="10" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="I104" s="5"/>
     </row>
     <row r="105" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="10" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B105" s="2" t="s">
         <v>9</v>
@@ -4831,22 +4828,22 @@
         <v>25</v>
       </c>
       <c r="E105" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F105" s="19" t="s">
         <v>14</v>
       </c>
       <c r="G105" s="33" t="s">
+        <v>168</v>
+      </c>
+      <c r="H105" s="10" t="s">
         <v>169</v>
-      </c>
-      <c r="H105" s="10" t="s">
-        <v>170</v>
       </c>
       <c r="I105" s="5"/>
     </row>
     <row r="106" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="10" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B106" s="2" t="s">
         <v>9</v>
@@ -4858,22 +4855,22 @@
         <v>25</v>
       </c>
       <c r="E106" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F106" s="19" t="s">
         <v>14</v>
       </c>
       <c r="G106" s="33" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H106" s="10" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="I106" s="5"/>
     </row>
     <row r="107" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="10" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B107" s="2" t="s">
         <v>9</v>
@@ -4885,22 +4882,22 @@
         <v>25</v>
       </c>
       <c r="E107" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F107" s="19" t="s">
         <v>14</v>
       </c>
       <c r="G107" s="33" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H107" s="10" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="I107" s="5"/>
     </row>
     <row r="108" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="10" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B108" s="2" t="s">
         <v>9</v>
@@ -4912,22 +4909,22 @@
         <v>25</v>
       </c>
       <c r="E108" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F108" s="19" t="s">
         <v>14</v>
       </c>
       <c r="G108" s="33" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H108" s="10" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="I108" s="5"/>
     </row>
     <row r="109" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="10" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B109" s="2" t="s">
         <v>9</v>
@@ -4939,22 +4936,22 @@
         <v>25</v>
       </c>
       <c r="E109" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F109" s="21" t="s">
         <v>14</v>
       </c>
       <c r="G109" s="34" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H109" s="10" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I109" s="5"/>
     </row>
     <row r="110" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="15" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B110" s="5"/>
       <c r="C110" s="5"/>
@@ -4967,7 +4964,7 @@
     </row>
     <row r="111" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="10" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B111" s="2" t="s">
         <v>9</v>
@@ -4979,22 +4976,22 @@
         <v>25</v>
       </c>
       <c r="E111" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F111" s="17" t="s">
         <v>14</v>
       </c>
       <c r="G111" s="35" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H111" s="10" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="I111" s="5"/>
     </row>
     <row r="112" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="10" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B112" s="2" t="s">
         <v>9</v>
@@ -5006,22 +5003,22 @@
         <v>25</v>
       </c>
       <c r="E112" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F112" s="19" t="s">
         <v>14</v>
       </c>
       <c r="G112" s="33" t="s">
+        <v>168</v>
+      </c>
+      <c r="H112" s="10" t="s">
         <v>169</v>
-      </c>
-      <c r="H112" s="10" t="s">
-        <v>170</v>
       </c>
       <c r="I112" s="5"/>
     </row>
     <row r="113" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="10" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B113" s="2" t="s">
         <v>9</v>
@@ -5033,22 +5030,22 @@
         <v>25</v>
       </c>
       <c r="E113" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F113" s="19" t="s">
         <v>14</v>
       </c>
       <c r="G113" s="33" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H113" s="10" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="I113" s="5"/>
     </row>
     <row r="114" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" s="10" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B114" s="2" t="s">
         <v>9</v>
@@ -5060,22 +5057,22 @@
         <v>25</v>
       </c>
       <c r="E114" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F114" s="19" t="s">
         <v>14</v>
       </c>
       <c r="G114" s="33" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H114" s="10" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="I114" s="5"/>
     </row>
     <row r="115" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" s="10" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B115" s="2" t="s">
         <v>9</v>
@@ -5087,22 +5084,22 @@
         <v>25</v>
       </c>
       <c r="E115" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F115" s="19" t="s">
         <v>14</v>
       </c>
       <c r="G115" s="33" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H115" s="10" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="I115" s="5"/>
     </row>
     <row r="116" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" s="10" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B116" s="2" t="s">
         <v>9</v>
@@ -5114,16 +5111,16 @@
         <v>25</v>
       </c>
       <c r="E116" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F116" s="21" t="s">
         <v>14</v>
       </c>
       <c r="G116" s="34" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H116" s="10" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I116" s="5"/>
     </row>
@@ -5140,7 +5137,7 @@
     </row>
     <row r="118" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" s="15" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B118" s="5"/>
       <c r="C118" s="5"/>
@@ -5153,7 +5150,7 @@
     </row>
     <row r="119" spans="1:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" s="36" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B119" s="2" t="s">
         <v>9</v>
@@ -5165,24 +5162,24 @@
         <v>25</v>
       </c>
       <c r="E119" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="F119" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="G119" s="37" t="s">
         <v>189</v>
       </c>
-      <c r="F119" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="G119" s="37" t="s">
+      <c r="H119" s="10" t="s">
+        <v>187</v>
+      </c>
+      <c r="I119" s="8" t="s">
         <v>190</v>
-      </c>
-      <c r="H119" s="10" t="s">
-        <v>188</v>
-      </c>
-      <c r="I119" s="8" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="120" spans="1:9" ht="13.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" s="10" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B120" s="2" t="s">
         <v>9</v>
@@ -5194,22 +5191,22 @@
         <v>25</v>
       </c>
       <c r="E120" s="38" t="s">
+        <v>192</v>
+      </c>
+      <c r="F120" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="G120" s="39" t="s">
+        <v>189</v>
+      </c>
+      <c r="H120" s="10" t="s">
         <v>193</v>
-      </c>
-      <c r="F120" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="G120" s="39" t="s">
-        <v>190</v>
-      </c>
-      <c r="H120" s="10" t="s">
-        <v>194</v>
       </c>
       <c r="I120" s="5"/>
     </row>
     <row r="121" spans="1:9" ht="13.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121" s="10" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B121" s="2" t="s">
         <v>9</v>
@@ -5221,22 +5218,22 @@
         <v>25</v>
       </c>
       <c r="E121" s="2" t="s">
-        <v>196</v>
+        <v>217</v>
       </c>
       <c r="F121" s="19" t="s">
         <v>14</v>
       </c>
       <c r="G121" s="39" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="H121" s="10" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="I121" s="5"/>
     </row>
     <row r="122" spans="1:9" ht="13.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" s="10" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B122" s="2" t="s">
         <v>9</v>
@@ -5248,24 +5245,24 @@
         <v>25</v>
       </c>
       <c r="E122" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="F122" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="G122" s="39" t="s">
+        <v>189</v>
+      </c>
+      <c r="H122" s="10" t="s">
+        <v>198</v>
+      </c>
+      <c r="I122" s="54" t="s">
         <v>199</v>
-      </c>
-      <c r="F122" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="G122" s="39" t="s">
-        <v>190</v>
-      </c>
-      <c r="H122" s="10" t="s">
-        <v>200</v>
-      </c>
-      <c r="I122" s="54" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="123" spans="1:9" ht="13.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" s="10" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B123" s="2" t="s">
         <v>9</v>
@@ -5277,22 +5274,22 @@
         <v>25</v>
       </c>
       <c r="E123" s="2" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="F123" s="19" t="s">
         <v>14</v>
       </c>
       <c r="G123" s="39" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="H123" s="10" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="I123" s="55"/>
     </row>
     <row r="124" spans="1:9" ht="13.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" s="10" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B124" s="2" t="s">
         <v>9</v>
@@ -5304,22 +5301,22 @@
         <v>25</v>
       </c>
       <c r="E124" s="2" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="F124" s="19" t="s">
         <v>14</v>
       </c>
       <c r="G124" s="39" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="H124" s="10" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="I124" s="55"/>
     </row>
     <row r="125" spans="1:9" ht="13.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" s="10" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B125" s="2" t="s">
         <v>9</v>
@@ -5331,22 +5328,22 @@
         <v>25</v>
       </c>
       <c r="E125" s="2" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="F125" s="19" t="s">
         <v>14</v>
       </c>
       <c r="G125" s="39" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="H125" s="10" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="I125" s="55"/>
     </row>
     <row r="126" spans="1:9" ht="13.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" s="10" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B126" s="2" t="s">
         <v>9</v>
@@ -5358,22 +5355,22 @@
         <v>25</v>
       </c>
       <c r="E126" s="2" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="F126" s="19" t="s">
         <v>14</v>
       </c>
       <c r="G126" s="39" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="H126" s="10" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="I126" s="55"/>
     </row>
     <row r="127" spans="1:9" ht="13.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" s="10" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B127" s="2" t="s">
         <v>9</v>
@@ -5385,16 +5382,16 @@
         <v>25</v>
       </c>
       <c r="E127" s="2" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="F127" s="19" t="s">
         <v>14</v>
       </c>
       <c r="G127" s="39" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="H127" s="10" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="I127" s="55"/>
     </row>
@@ -5501,11 +5498,11 @@
     <row r="7" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="42"/>
       <c r="B7" s="28" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C7" s="47"/>
       <c r="D7" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E7" s="48">
         <v>8947039344</v>
@@ -5514,11 +5511,11 @@
     <row r="8" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="42"/>
       <c r="B8" s="28" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C8" s="47"/>
       <c r="D8" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E8" s="48">
         <v>5722478949</v>
@@ -5527,11 +5524,11 @@
     <row r="9" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="42"/>
       <c r="B9" s="28" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C9" s="47"/>
       <c r="D9" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E9" s="48">
         <v>1766681427</v>
@@ -5540,7 +5537,7 @@
     <row r="10" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="42"/>
       <c r="B10" s="28" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C10" s="47"/>
       <c r="D10" s="2" t="s">
@@ -5553,7 +5550,7 @@
     <row r="11" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="42"/>
       <c r="B11" s="28" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C11" s="47"/>
       <c r="D11" s="2" t="s">
@@ -5566,11 +5563,11 @@
     <row r="12" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="42"/>
       <c r="B12" s="28" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C12" s="47"/>
       <c r="D12" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E12" s="48">
         <v>2379307763</v>
@@ -5579,11 +5576,11 @@
     <row r="13" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="42"/>
       <c r="B13" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C13" s="43"/>
       <c r="D13" s="49" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E13" s="45">
         <v>45145075</v>
@@ -5592,11 +5589,11 @@
     <row r="14" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="42"/>
       <c r="B14" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C14" s="43"/>
       <c r="D14" s="44" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E14" s="45">
         <v>2334162688</v>
@@ -5605,24 +5602,24 @@
     <row r="15" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="42"/>
       <c r="B15" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C15" s="43"/>
       <c r="D15" s="44" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E15" s="44" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="42"/>
       <c r="B16" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C16" s="43"/>
       <c r="D16" s="44" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E16" s="45">
         <v>2334162688</v>
@@ -5631,11 +5628,11 @@
     <row r="17" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="42"/>
       <c r="B17" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C17" s="43"/>
       <c r="D17" s="44" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E17" s="45">
         <v>815650000</v>
@@ -5656,7 +5653,7 @@
       <c r="C19" s="43"/>
       <c r="D19" s="40"/>
       <c r="E19" s="44" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5665,7 +5662,7 @@
       <c r="C20" s="43"/>
       <c r="D20" s="40"/>
       <c r="E20" s="44" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated Form 8 Points
</commit_message>
<xml_diff>
--- a/Config Files/FORM-8(ANNUAL)_nodes_config.xlsx
+++ b/Config Files/FORM-8(ANNUAL)_nodes_config.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mns-admin\Documents\Python\Config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MCA Portal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11D3020D-4551-4060-AF56-27C790302483}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6E6CAAC-C810-4FAF-A670-6CCDC2B69C62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="931" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="931" uniqueCount="216">
   <si>
     <t>Field_Name</t>
   </si>
@@ -596,16 +596,10 @@
     <t>if it is auditor then only capture below fields</t>
   </si>
   <si>
-    <t>auditor_name</t>
-  </si>
-  <si>
     <t>NAME_DPAR_AR_AU</t>
   </si>
   <si>
     <t>name</t>
-  </si>
-  <si>
-    <t>membership_number</t>
   </si>
   <si>
     <t>id</t>
@@ -2188,8 +2182,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I127"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A98" workbookViewId="0">
-      <selection activeCell="E126" sqref="E126"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A110" workbookViewId="0">
+      <selection activeCell="E121" sqref="E121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5179,7 +5173,7 @@
     </row>
     <row r="120" spans="1:9" ht="13.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" s="10" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B120" s="2" t="s">
         <v>9</v>
@@ -5191,7 +5185,7 @@
         <v>25</v>
       </c>
       <c r="E120" s="38" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F120" s="19" t="s">
         <v>14</v>
@@ -5200,13 +5194,13 @@
         <v>189</v>
       </c>
       <c r="H120" s="10" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I120" s="5"/>
     </row>
     <row r="121" spans="1:9" ht="13.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121" s="10" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B121" s="2" t="s">
         <v>9</v>
@@ -5218,7 +5212,7 @@
         <v>25</v>
       </c>
       <c r="E121" s="2" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F121" s="19" t="s">
         <v>14</v>
@@ -5227,13 +5221,13 @@
         <v>189</v>
       </c>
       <c r="H121" s="10" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="I121" s="5"/>
     </row>
     <row r="122" spans="1:9" ht="13.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" s="10" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B122" s="2" t="s">
         <v>9</v>
@@ -5245,7 +5239,7 @@
         <v>25</v>
       </c>
       <c r="E122" s="2" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="F122" s="19" t="s">
         <v>14</v>
@@ -5254,15 +5248,15 @@
         <v>189</v>
       </c>
       <c r="H122" s="10" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="I122" s="54" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="123" spans="1:9" ht="13.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" s="10" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B123" s="2" t="s">
         <v>9</v>
@@ -5274,7 +5268,7 @@
         <v>25</v>
       </c>
       <c r="E123" s="2" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F123" s="19" t="s">
         <v>14</v>
@@ -5283,13 +5277,13 @@
         <v>189</v>
       </c>
       <c r="H123" s="10" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="I123" s="55"/>
     </row>
     <row r="124" spans="1:9" ht="13.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" s="10" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B124" s="2" t="s">
         <v>9</v>
@@ -5301,7 +5295,7 @@
         <v>25</v>
       </c>
       <c r="E124" s="2" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="F124" s="19" t="s">
         <v>14</v>
@@ -5310,13 +5304,13 @@
         <v>189</v>
       </c>
       <c r="H124" s="10" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="I124" s="55"/>
     </row>
     <row r="125" spans="1:9" ht="13.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" s="10" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B125" s="2" t="s">
         <v>9</v>
@@ -5328,7 +5322,7 @@
         <v>25</v>
       </c>
       <c r="E125" s="2" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="F125" s="19" t="s">
         <v>14</v>
@@ -5337,13 +5331,13 @@
         <v>189</v>
       </c>
       <c r="H125" s="10" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="I125" s="55"/>
     </row>
     <row r="126" spans="1:9" ht="13.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" s="10" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B126" s="2" t="s">
         <v>9</v>
@@ -5355,7 +5349,7 @@
         <v>25</v>
       </c>
       <c r="E126" s="2" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="F126" s="19" t="s">
         <v>14</v>
@@ -5364,13 +5358,13 @@
         <v>189</v>
       </c>
       <c r="H126" s="10" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="I126" s="55"/>
     </row>
     <row r="127" spans="1:9" ht="13.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" s="10" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B127" s="2" t="s">
         <v>9</v>
@@ -5382,7 +5376,7 @@
         <v>25</v>
       </c>
       <c r="E127" s="2" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="F127" s="19" t="s">
         <v>14</v>
@@ -5391,7 +5385,7 @@
         <v>189</v>
       </c>
       <c r="H127" s="10" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="I127" s="55"/>
     </row>
@@ -5498,7 +5492,7 @@
     <row r="7" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="42"/>
       <c r="B7" s="28" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C7" s="47"/>
       <c r="D7" s="2" t="s">
@@ -5511,7 +5505,7 @@
     <row r="8" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="42"/>
       <c r="B8" s="28" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C8" s="47"/>
       <c r="D8" s="2" t="s">
@@ -5524,7 +5518,7 @@
     <row r="9" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="42"/>
       <c r="B9" s="28" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C9" s="47"/>
       <c r="D9" s="2" t="s">
@@ -5537,7 +5531,7 @@
     <row r="10" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="42"/>
       <c r="B10" s="28" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C10" s="47"/>
       <c r="D10" s="2" t="s">
@@ -5550,7 +5544,7 @@
     <row r="11" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="42"/>
       <c r="B11" s="28" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C11" s="47"/>
       <c r="D11" s="2" t="s">
@@ -5563,7 +5557,7 @@
     <row r="12" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="42"/>
       <c r="B12" s="28" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C12" s="47"/>
       <c r="D12" s="2" t="s">
@@ -5609,7 +5603,7 @@
         <v>136</v>
       </c>
       <c r="E15" s="44" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5653,7 +5647,7 @@
       <c r="C19" s="43"/>
       <c r="D19" s="40"/>
       <c r="E19" s="44" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5662,7 +5656,7 @@
       <c r="C20" s="43"/>
       <c r="D20" s="40"/>
       <c r="E20" s="44" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>